<commit_message>
pushing the code in git
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E2058C79-198B-4E16-980A-57DDDB2C8212}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="2"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Companies" sheetId="2" r:id="rId2"/>
     <sheet name="Deals" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:P11"/>
 </workbook>
 </file>
 
@@ -255,7 +257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,6 +307,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -352,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,9 +390,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,6 +442,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,7 +634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -666,10 +705,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -829,10 +868,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding code for Cases functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E2058C79-198B-4E16-980A-57DDDB2C8212}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Companies" sheetId="2" r:id="rId2"/>
     <sheet name="Deals" sheetId="3" r:id="rId3"/>
+    <sheet name="Cases" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="90">
   <si>
     <t>title</t>
   </si>
@@ -252,12 +251,48 @@
   </si>
   <si>
     <t>5000</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>CaseTitle1</t>
+  </si>
+  <si>
+    <t>CaseTitle2</t>
+  </si>
+  <si>
+    <t>Awaiting input</t>
+  </si>
+  <si>
+    <t>Enquiring</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>Business Support</t>
+  </si>
+  <si>
+    <t>Complaint</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>zzzx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,26 +425,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,23 +460,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -634,7 +635,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -705,11 +706,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,11 +869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,4 +979,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added code for New Word Mail Merge Template functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="5"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Cases" sheetId="4" r:id="rId4"/>
     <sheet name="Calls" sheetId="5" r:id="rId5"/>
     <sheet name="Docs" sheetId="6" r:id="rId6"/>
+    <sheet name="Templates" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
   <si>
     <t>title</t>
   </si>
@@ -388,6 +389,30 @@
   </si>
   <si>
     <t>zyxwvy</t>
+  </si>
+  <si>
+    <t>Template1</t>
+  </si>
+  <si>
+    <t>Template1 description</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>Template 1 tags</t>
+  </si>
+  <si>
+    <t>Template2</t>
+  </si>
+  <si>
+    <t>Template2 description</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>Template 2 tags</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1334,4 +1359,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added code for Multi Doc Upload functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="6"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Calls" sheetId="5" r:id="rId5"/>
     <sheet name="Docs" sheetId="6" r:id="rId6"/>
     <sheet name="Templates" sheetId="7" r:id="rId7"/>
+    <sheet name="MultiDocs" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
   <si>
     <t>title</t>
   </si>
@@ -413,6 +414,51 @@
   </si>
   <si>
     <t>Template 2 tags</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>Root directory</t>
+  </si>
+  <si>
+    <t>Word Templates</t>
+  </si>
+  <si>
+    <t>contact1</t>
+  </si>
+  <si>
+    <t>contact2</t>
+  </si>
+  <si>
+    <t>company1</t>
+  </si>
+  <si>
+    <t>company2</t>
+  </si>
+  <si>
+    <t>prospect1</t>
+  </si>
+  <si>
+    <t>prospect2</t>
+  </si>
+  <si>
+    <t>task1</t>
+  </si>
+  <si>
+    <t>task2</t>
+  </si>
+  <si>
+    <t>case1</t>
+  </si>
+  <si>
+    <t>case2</t>
+  </si>
+  <si>
+    <t>tag1</t>
+  </si>
+  <si>
+    <t>tag2</t>
   </si>
 </sst>
 </file>
@@ -1365,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,4 +1468,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added code for New Task functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="7"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="Docs" sheetId="6" r:id="rId6"/>
     <sheet name="Templates" sheetId="7" r:id="rId7"/>
     <sheet name="MultiDocs" sheetId="8" r:id="rId8"/>
+    <sheet name="FeedbackForms" sheetId="9" r:id="rId9"/>
+    <sheet name="Tasks" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
   <si>
     <t>title</t>
   </si>
@@ -459,16 +461,129 @@
   </si>
   <si>
     <t>tag2</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>reportEmail</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>welcomeMessage</t>
+  </si>
+  <si>
+    <t>confirmationMessage</t>
+  </si>
+  <si>
+    <t>Form title 1</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Form 1 description</t>
+  </si>
+  <si>
+    <t>Form 1 welcome message</t>
+  </si>
+  <si>
+    <t>Form1 confirmation message</t>
+  </si>
+  <si>
+    <t>Form title 2</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>def@gmail.com</t>
+  </si>
+  <si>
+    <t>Form 2 description</t>
+  </si>
+  <si>
+    <t>Form 2 welcome message</t>
+  </si>
+  <si>
+    <t>Form2 confirmation message</t>
+  </si>
+  <si>
+    <t>autoextend</t>
+  </si>
+  <si>
+    <t>completionpercentage</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>Task2</t>
+  </si>
+  <si>
+    <t>Extend deadline by 1 day</t>
+  </si>
+  <si>
+    <t>Extend deadline by 30 days</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Call</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>deal1</t>
+  </si>
+  <si>
+    <t>deal2</t>
+  </si>
+  <si>
+    <t>tagdesc1</t>
+  </si>
+  <si>
+    <t>tagdesc2</t>
+  </si>
+  <si>
+    <t>identifier1</t>
+  </si>
+  <si>
+    <t>identifier2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -497,15 +612,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -877,6 +995,148 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" t="s">
+        <v>135</v>
+      </c>
+      <c r="L3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
@@ -1474,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1555,4 +1815,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added code for Create New Alert functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="9"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="MultiDocs" sheetId="8" r:id="rId8"/>
     <sheet name="FeedbackForms" sheetId="9" r:id="rId9"/>
     <sheet name="Tasks" sheetId="10" r:id="rId10"/>
+    <sheet name="Alerts" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="195">
   <si>
     <t>title</t>
   </si>
@@ -566,6 +567,48 @@
   </si>
   <si>
     <t>identifier2</t>
+  </si>
+  <si>
+    <t>AlertSendMode</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>[O]wner</t>
+  </si>
+  <si>
+    <t>[S]pecific User (select below)</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Ownership Changed</t>
+  </si>
+  <si>
+    <t>Note Added</t>
+  </si>
+  <si>
+    <t>Email Alert</t>
+  </si>
+  <si>
+    <t>Text Message Alert</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -999,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,6 +1173,76 @@
       </c>
       <c r="M3" t="s">
         <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1822,7 +1935,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added code for Create New Message functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="10"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23004" windowHeight="12888" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="FeedbackForms" sheetId="9" r:id="rId9"/>
     <sheet name="Tasks" sheetId="10" r:id="rId10"/>
     <sheet name="Alerts" sheetId="11" r:id="rId11"/>
+    <sheet name="Messages" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="201">
   <si>
     <t>title</t>
   </si>
@@ -609,6 +610,24 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>new message 1</t>
+  </si>
+  <si>
+    <t>new message 1 text</t>
+  </si>
+  <si>
+    <t>new message 2</t>
+  </si>
+  <si>
+    <t>new message 2 text</t>
   </si>
 </sst>
 </file>
@@ -1184,14 +1203,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1243,6 +1263,47 @@
       </c>
       <c r="E3" t="s">
         <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>